<commit_message>
Updates to project and stuff
</commit_message>
<xml_diff>
--- a/.informations/ScénarioUtilisation/AlexandreParent.xlsx
+++ b/.informations/ScénarioUtilisation/AlexandreParent.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="19">
   <si>
     <t>Titre</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Création de plan</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur connecté, je veux éditer un plan préexistent pour l’adapter à mes besoins.</t>
   </si>
 </sst>
 </file>
@@ -658,7 +661,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B5" sqref="B5:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +686,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Scenarios and models updates
</commit_message>
<xml_diff>
--- a/.informations/ScénarioUtilisation/AlexandreParent.xlsx
+++ b/.informations/ScénarioUtilisation/AlexandreParent.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Scénario 6" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="41">
   <si>
     <t>Titre</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Suppression de projets</t>
   </si>
   <si>
-    <t>En tant qu'utilisateur connecté, l'utilisateur veux supprimer ses projets rapidement depuis l'écran principal.</t>
-  </si>
-  <si>
     <t>Les projets deviennent grisés et supprimable.</t>
   </si>
   <si>
@@ -73,13 +70,82 @@
     <t>Les projets sont sélectionnés et mis en surbrillance.</t>
   </si>
   <si>
-    <t>En tant qu'utilisateur connecté, je veux créer un plan de clôture.</t>
-  </si>
-  <si>
     <t>Création de plan</t>
   </si>
   <si>
-    <t>En tant qu'utilisateur connecté, je veux éditer un plan préexistent pour l’adapter à mes besoins.</t>
+    <t>En tant qu'utilisateur connecté, l'utilisateur veux éditer un plan préexistent pour l’adapter à ses besoins.</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur connecté, l'utilisateur veut supprimer ses projets rapidement depuis l'écran principal.</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur connecté, l'utilisateur veut créer un plan de clôture.</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur connecté, lorsqu'il édite un plan, l'utilisateur veut pouvoir ajouter des éléments au plan et les déplacer.</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur connecté, lorsqu'il édite un plan, l'utilisateur veut pouvoir modifier la taille des éléments et la forme des éléments de mon plan.</t>
+  </si>
+  <si>
+    <t>Clique sur le bouton de création de projet.</t>
+  </si>
+  <si>
+    <t>Une fenêtre modale avec le champs "Nom" apparait.</t>
+  </si>
+  <si>
+    <t>Remplis le champ "Nom".</t>
+  </si>
+  <si>
+    <t>"Ma clôture"</t>
+  </si>
+  <si>
+    <t>Clique sur "" ou appuie sur Entrée.</t>
+  </si>
+  <si>
+    <t>Crée le projet.</t>
+  </si>
+  <si>
+    <t>Clique sur l'un des projets sur la page principale.</t>
+  </si>
+  <si>
+    <t>Redirige sur la fenêtre d'édition du projet.</t>
+  </si>
+  <si>
+    <t>Scénario 8; 0-1</t>
+  </si>
+  <si>
+    <t>Le matériaux est sélectionnée.</t>
+  </si>
+  <si>
+    <t>Clique sur une forme.</t>
+  </si>
+  <si>
+    <t>Clique sur un matériau.</t>
+  </si>
+  <si>
+    <t>La forme est sélectionnée.</t>
+  </si>
+  <si>
+    <t>Clique dans l'écran d'édition.</t>
+  </si>
+  <si>
+    <t>Génère une forme dans le plan aux coordonnées du clic.</t>
+  </si>
+  <si>
+    <t>Déplace la forme jusqu'à la nouvelle position.</t>
+  </si>
+  <si>
+    <t>Clique sur "Sauvegarder".</t>
+  </si>
+  <si>
+    <t>Persiste le projet.</t>
+  </si>
+  <si>
+    <t>Clique sur la forme dans l'écran d'édition et la drag.</t>
+  </si>
+  <si>
+    <t>Clique sur la forme dans l'écran d'édition.</t>
   </si>
 </sst>
 </file>
@@ -419,7 +485,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +510,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -484,12 +550,12 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
@@ -497,12 +563,12 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
@@ -510,11 +576,11 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="3"/>
     </row>
@@ -523,10 +589,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -540,7 +606,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +623,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
@@ -565,7 +631,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -605,50 +671,46 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="3"/>
+      <c r="D8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -660,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,7 +748,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -726,50 +788,32 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>3</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="3"/>
+      <c r="D8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -779,10 +823,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,7 +851,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -832,64 +876,75 @@
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>11</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -902,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +983,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -953,14 +1008,14 @@
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
@@ -968,38 +1023,27 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1007,10 +1051,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>